<commit_message>
Updates as of May 16, 2025
</commit_message>
<xml_diff>
--- a/2025 Representatives.xlsx
+++ b/2025 Representatives.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\USA Dance\Ranking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e238e71ce846790e/Documents/USA Dance/Ranking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A737E1AE-466C-4CE3-BCD2-1CD6571AAA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{A737E1AE-466C-4CE3-BCD2-1CD6571AAA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B0F7371-7B90-49AC-BF29-6C193E6DE5D6}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="96" windowWidth="14952" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="492" yWindow="0" windowWidth="21660" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Couples" sheetId="1" r:id="rId1"/>
     <sheet name="Events" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Couples!$A$1:$L$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Couples!$A$1:$L$155</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="209">
   <si>
     <t>Date</t>
   </si>
@@ -814,34 +814,6 @@
   </cellStyles>
   <dxfs count="32">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
@@ -908,6 +880,34 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1373,10 +1373,10 @@
   <dimension ref="A1:L155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E63" sqref="E63"/>
+      <selection pane="bottomRight" activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>11</v>
@@ -1777,7 +1777,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>12</v>
@@ -2020,17 +2020,23 @@
       <c r="D24" s="13">
         <v>5</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G24" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(F24,Events!A:E,2,FALSE)),"",IF(ISBLANK(VLOOKUP(F24,Events!A:E,2,FALSE)),"",VLOOKUP(F24,Events!A:E,2,FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H24" s="7" t="str">
+        <v>Elblag - Poland</v>
+      </c>
+      <c r="H24" s="7">
         <f>IF(ISNA(VLOOKUP(F24,Events!A:E,3,FALSE)),"",IF(ISBLANK(VLOOKUP(F24,Events!A:E,3,FALSE)),"",VLOOKUP(F24,Events!A:E,3,FALSE)))</f>
-        <v/>
-      </c>
-      <c r="I24" s="3"/>
+        <v>45955</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="J24" s="3"/>
       <c r="K24" s="13"/>
       <c r="L24" s="3"/>
@@ -2079,22 +2085,17 @@
         <v>3</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>13</v>
+        <v>202</v>
       </c>
       <c r="G26" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(F26,Events!A:E,2,FALSE)),"",IF(ISBLANK(VLOOKUP(F26,Events!A:E,2,FALSE)),"",VLOOKUP(F26,Events!A:E,2,FALSE)))</f>
-        <v>Elblag - Poland</v>
-      </c>
-      <c r="H26" s="7">
+        <v/>
+      </c>
+      <c r="H26" s="7" t="str">
         <f>IF(ISNA(VLOOKUP(F26,Events!A:E,3,FALSE)),"",IF(ISBLANK(VLOOKUP(F26,Events!A:E,3,FALSE)),"",VLOOKUP(F26,Events!A:E,3,FALSE)))</f>
-        <v>45955</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v/>
+      </c>
+      <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="13"/>
       <c r="L26" s="3"/>
@@ -2192,7 +2193,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>14</v>
@@ -2417,7 +2418,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>20</v>
@@ -2611,22 +2612,18 @@
         <v>2</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="F45" s="3"/>
       <c r="G45" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(F45,Events!A:E,2,FALSE)),"",IF(ISBLANK(VLOOKUP(F45,Events!A:E,2,FALSE)),"",VLOOKUP(F45,Events!A:E,2,FALSE)))</f>
-        <v>Bremen - Germany</v>
-      </c>
-      <c r="H45" s="7">
+        <v/>
+      </c>
+      <c r="H45" s="7" t="str">
         <f>IF(ISNA(VLOOKUP(F45,Events!A:E,3,FALSE)),"",IF(ISBLANK(VLOOKUP(F45,Events!A:E,3,FALSE)),"",VLOOKUP(F45,Events!A:E,3,FALSE)))</f>
-        <v>45815</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v/>
+      </c>
+      <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="13"/>
       <c r="L45" s="3"/>
@@ -2915,7 +2912,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
@@ -4985,7 +4982,7 @@
         <v>3</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>31</v>
@@ -5583,35 +5580,35 @@
       <c r="L155" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L146" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A17:A19 A28:A29 A31:A32 A34:A37 A39:A43 A45:A46 A47:B48 A49:A63 A81:A97 A99:A155 A2:A8 A10 A12:A13 A21:A23 A25 A65:A79">
+  <autoFilter ref="A1:L155" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A2:A8 A10 A12:A13 A17:A19 A21:A23 A25 A28:A29 A31:A32 A34:A37 A39:A43 A45:A46 A47:B48 A49:A63 A65:A79 A81:A97 A99:A155">
     <cfRule type="expression" dxfId="31" priority="25">
       <formula>OR(I2="Place",I2="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
-    <cfRule type="expression" dxfId="30" priority="28">
-      <formula>OR(I81="Place",I81="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A98">
-    <cfRule type="expression" dxfId="29" priority="32">
-      <formula>OR(I100="Place",I100="Rank",#REF!="Place",#REF!="Rank")</formula>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="30" priority="65">
+      <formula>OR(I11="Place",I11="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="28" priority="35">
+    <cfRule type="expression" dxfId="29" priority="35">
       <formula>OR(I16="Place",I16="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20 A15">
-    <cfRule type="expression" dxfId="27" priority="3">
+  <conditionalFormatting sqref="A15 A20">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>OR(I14="Place",I14="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="26" priority="9">
+    <cfRule type="expression" dxfId="27" priority="9">
       <formula>OR(I26="Place",I26="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="expression" dxfId="26" priority="69">
+      <formula>OR(I24="Place",I24="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
@@ -5634,104 +5631,104 @@
       <formula>OR(I48="Place",I48="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A80">
+    <cfRule type="expression" dxfId="21" priority="28">
+      <formula>OR(I81="Place",I81="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98">
+    <cfRule type="expression" dxfId="20" priority="32">
+      <formula>OR(I100="Place",I100="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A64:B64">
-    <cfRule type="expression" dxfId="21" priority="63">
+    <cfRule type="expression" dxfId="19" priority="63">
       <formula>OR(#REF!="Place",#REF!="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B19 B28:B29 B31:B32 B34:B37 B39:B43 B45:B46 B49:B63 B81:B97 B99:B155 B2:B8 B10 B12:B13 B21:B23 B25 B65:B79">
-    <cfRule type="expression" dxfId="20" priority="26">
+  <conditionalFormatting sqref="B2:B8 B10 B12:B13 B17:B19 B21:B23 B25 B28:B29 B31:B32 B34:B37 B39:B43 B45:B46 B49:B63 B65:B79 B81:B97 B99:B155">
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>OR(I2="Place",I2="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="17" priority="67">
+      <formula>OR(I11="Place",I11="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="expression" dxfId="16" priority="36">
+      <formula>OR(I16="Place",I16="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15 B20">
+    <cfRule type="expression" dxfId="15" priority="4">
+      <formula>OR(I14="Place",I14="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>OR(I26="Place",I26="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="13" priority="71">
+      <formula>OR(I24="Place",I24="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>OR(I32="Place",I32="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="expression" dxfId="11" priority="6">
+      <formula>OR(I30="Place",I30="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>OR(I40="Place",I40="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" dxfId="9" priority="44">
+      <formula>OR(I48="Place",I48="Rank",#REF!="Place",#REF!="Rank")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B80">
-    <cfRule type="expression" dxfId="19" priority="30">
+    <cfRule type="expression" dxfId="8" priority="30">
       <formula>OR(I81="Place",I81="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="expression" dxfId="18" priority="34">
+    <cfRule type="expression" dxfId="7" priority="34">
       <formula>OR(I100="Place",I100="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="17" priority="36">
-      <formula>OR(I16="Place",I16="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20 B15">
-    <cfRule type="expression" dxfId="16" priority="4">
-      <formula>OR(I14="Place",I14="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="15" priority="10">
-      <formula>OR(I26="Place",I26="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="14" priority="8">
-      <formula>OR(I32="Place",I32="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="13" priority="6">
-      <formula>OR(I30="Place",I30="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="12" priority="2">
-      <formula>OR(I40="Place",I40="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="11" priority="44">
-      <formula>OR(I48="Place",I48="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
       <formula>"Sent"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="15" operator="equal">
       <formula>"Required"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="24" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H155">
-    <cfRule type="cellIs" dxfId="6" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>TODAY()</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="5" priority="17" stopIfTrue="1" timePeriod="thisMonth">
+    <cfRule type="timePeriod" dxfId="1" priority="17" stopIfTrue="1" timePeriod="thisMonth">
       <formula>AND(MONTH(H2)=MONTH(TODAY()),YEAR(H2)=YEAR(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="4" priority="20" stopIfTrue="1" timePeriod="nextMonth">
+    <cfRule type="timePeriod" dxfId="0" priority="20" stopIfTrue="1" timePeriod="nextMonth">
       <formula>AND(MONTH(H2)=MONTH(EDATE(TODAY(),0+1)),YEAR(H2)=YEAR(EDATE(TODAY(),0+1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="3" priority="65">
-      <formula>OR(I11="Place",I11="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="2" priority="67">
-      <formula>OR(I11="Place",I11="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="expression" dxfId="1" priority="69">
-      <formula>OR(I24="Place",I24="Rank",#REF!="Place",#REF!="Rank")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="0" priority="71">
-      <formula>OR(I24="Place",I24="Rank",#REF!="Place",#REF!="Rank")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -5751,13 +5748,13 @@
           <x14:formula1>
             <xm:f>Events!$A$6:$A$53</xm:f>
           </x14:formula1>
-          <xm:sqref>F155 F153 F151 F143 F146 F86 F141 F139 F137 F135 F132 F128 F124 F117 F112 F105 F103 F97 F90 F83 F76 F74 F148 F62 F55 F3 F43 F39 F35 F28 F22:F24 F19 F13:F14 F8:F9 F5 F1 F50 F72 F68 F70 F26</xm:sqref>
+          <xm:sqref>F155 F153 F151 F143 F146 F86 F141 F139 F137 F135 F132 F128 F124 F117 F112 F105 F103 F97 F90 F83 F76 F74 F148 F62 F55 F3 F43 F39 F35 F28 F19 F13:F14 F8:F9 F5 F1 F50 F72 F68 F70 F22:F24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FA1A5BDD-BDAF-4F80-8DDA-7A1604F21FB4}">
           <x14:formula1>
             <xm:f>Events!$A$6:$A$55</xm:f>
           </x14:formula1>
-          <xm:sqref>F154 F152 F149:F150 F147 F144:F145 F142 F140 F138 F136 F23:F27 F106:F111 F125:F127 F118:F123 F113:F116 F98:F102 F104 F36:F38 F91:F96 F87:F89 F84:F85 F75 F73 F71 F63:F67 F56:F61 F51:F54 F44:F49 F40:F42 F133:F134 F29:F34 F20:F21 F77:F82 F69 F9:F12 F14:F18 F129:F131</xm:sqref>
+          <xm:sqref>F154 F152 F149:F150 F147 F144:F145 F142 F140 F138 F136 F106:F111 F125:F127 F118:F123 F113:F116 F98:F102 F104 F36:F38 F91:F96 F87:F89 F84:F85 F75 F73 F71 F63:F67 F56:F61 F51:F54 F129:F131 F40:F42 F133:F134 F29:F34 F20:F21 F77:F82 F69 F9:F12 F14:F18 F44:F49 F27 F23:F25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BAD7700-9E34-42C3-AD29-A8CD551F0849}">
           <x14:formula1>
@@ -5775,8 +5772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added Adult Showcase World Championship representatives
</commit_message>
<xml_diff>
--- a/2025 Representatives.xlsx
+++ b/2025 Representatives.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e238e71ce846790e/Documents/USA Dance/Ranking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{A737E1AE-466C-4CE3-BCD2-1CD6571AAA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B0F7371-7B90-49AC-BF29-6C193E6DE5D6}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{A737E1AE-466C-4CE3-BCD2-1CD6571AAA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BDD9794-F98A-4A26-89BB-086CED2B22E4}"/>
   <bookViews>
-    <workbookView xWindow="492" yWindow="0" windowWidth="21660" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1368" yWindow="0" windowWidth="21672" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Couples" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="209">
   <si>
     <t>Date</t>
   </si>
@@ -1083,6 +1083,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -1373,10 +1377,10 @@
   <dimension ref="A1:L155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E130" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E129" sqref="E129"/>
+      <selection pane="bottomRight" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3120,7 +3124,7 @@
       </c>
       <c r="H63" s="7">
         <f>IF(ISNA(VLOOKUP(F63,Events!A:E,3,FALSE)),"",IF(ISBLANK(VLOOKUP(F63,Events!A:E,3,FALSE)),"",VLOOKUP(F63,Events!A:E,3,FALSE)))</f>
-        <v>45942</v>
+        <v>45948</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>7</v>
@@ -3154,7 +3158,7 @@
       </c>
       <c r="H64" s="7">
         <f>IF(ISNA(VLOOKUP(F64,Events!A:E,3,FALSE)),"",IF(ISBLANK(VLOOKUP(F64,Events!A:E,3,FALSE)),"",VLOOKUP(F64,Events!A:E,3,FALSE)))</f>
-        <v>45942</v>
+        <v>45948</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>6</v>
@@ -3379,17 +3383,19 @@
       <c r="D73" s="13">
         <v>1</v>
       </c>
-      <c r="E73" s="3"/>
+      <c r="E73" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="F73" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G73" s="3" t="str">
         <f>IF(ISNA(VLOOKUP(F73,Events!A:E,2,FALSE)),"",IF(ISBLANK(VLOOKUP(F73,Events!A:E,2,FALSE)),"",VLOOKUP(F73,Events!A:E,2,FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H73" s="7" t="str">
+        <v>Brno - Czechia</v>
+      </c>
+      <c r="H73" s="7">
         <f>IF(ISNA(VLOOKUP(F73,Events!A:E,3,FALSE)),"",IF(ISBLANK(VLOOKUP(F73,Events!A:E,3,FALSE)),"",VLOOKUP(F73,Events!A:E,3,FALSE)))</f>
-        <v/>
+        <v>45946</v>
       </c>
       <c r="I73" s="3" t="s">
         <v>7</v>
@@ -5772,8 +5778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6023,7 +6029,7 @@
         <v>126</v>
       </c>
       <c r="C16" s="8">
-        <v>45942</v>
+        <v>45948</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -6053,7 +6059,12 @@
       <c r="A18" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="B18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="8">
+        <v>45946</v>
+      </c>
       <c r="D18">
         <v>1</v>
       </c>

</xml_diff>